<commit_message>
update settingfiles for 1205 midi-generate
</commit_message>
<xml_diff>
--- a/CompileThemeStyle.xlsx
+++ b/CompileThemeStyle.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="result" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="quantities" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="result" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="quantities" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
 </workbook>
@@ -399,7 +399,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -535,7 +535,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1620,18 +1626,18 @@
     <col width="10" customWidth="1" style="40" min="6" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25.9" customHeight="1" s="47">
+    <row r="1" ht="25.9" customHeight="1" s="49">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>MusicEngine_CompileTheme-Style_0724</t>
         </is>
       </c>
-      <c r="B1" s="48" t="n"/>
-      <c r="C1" s="48" t="n"/>
-      <c r="D1" s="48" t="n"/>
-      <c r="E1" s="49" t="n"/>
-    </row>
-    <row r="2" ht="18.6" customHeight="1" s="47">
+      <c r="B1" s="50" t="n"/>
+      <c r="C1" s="50" t="n"/>
+      <c r="D1" s="50" t="n"/>
+      <c r="E1" s="51" t="n"/>
+    </row>
+    <row r="2" ht="18.6" customHeight="1" s="49">
       <c r="A2" s="6" t="inlineStr">
         <is>
           <t>CompileTheme</t>
@@ -1658,7 +1664,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.6" customHeight="1" s="47">
+    <row r="3" ht="18.6" customHeight="1" s="49">
       <c r="A3" s="8" t="inlineStr">
         <is>
           <t>Cafe4</t>
@@ -1683,7 +1689,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18.4" customHeight="1" s="47">
+    <row r="4" ht="18.4" customHeight="1" s="49">
       <c r="A4" s="13" t="inlineStr">
         <is>
           <t>Cafe4</t>
@@ -1708,7 +1714,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="18.4" customHeight="1" s="47">
+    <row r="5" ht="18.4" customHeight="1" s="49">
       <c r="A5" s="13" t="inlineStr">
         <is>
           <t>Cafe(Up)1</t>
@@ -1733,7 +1739,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="18.4" customHeight="1" s="47">
+    <row r="6" ht="18.4" customHeight="1" s="49">
       <c r="A6" s="13" t="inlineStr">
         <is>
           <t>Cafe(Up)1</t>
@@ -1758,7 +1764,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.4" customHeight="1" s="47">
+    <row r="7" ht="18.4" customHeight="1" s="49">
       <c r="A7" s="13" t="inlineStr">
         <is>
           <t>Cafe(Slow)1</t>
@@ -1783,7 +1789,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="18.4" customHeight="1" s="47">
+    <row r="8" ht="18.4" customHeight="1" s="49">
       <c r="A8" s="13" t="inlineStr">
         <is>
           <t>Cafe(Slow)1</t>
@@ -1808,7 +1814,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="18.4" customHeight="1" s="47">
+    <row r="9" ht="18.4" customHeight="1" s="49">
       <c r="A9" s="13" t="inlineStr">
         <is>
           <t>Morning1</t>
@@ -1833,7 +1839,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="18.4" customHeight="1" s="47">
+    <row r="10" ht="18.4" customHeight="1" s="49">
       <c r="A10" s="13" t="inlineStr">
         <is>
           <t>Morning1</t>
@@ -1858,7 +1864,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="18.4" customHeight="1" s="47">
+    <row r="11" ht="18.4" customHeight="1" s="49">
       <c r="A11" s="13" t="inlineStr">
         <is>
           <t>Morning1</t>
@@ -1883,7 +1889,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="18.4" customHeight="1" s="47">
+    <row r="12" ht="18.4" customHeight="1" s="49">
       <c r="A12" s="13" t="inlineStr">
         <is>
           <t>Night1</t>
@@ -1908,7 +1914,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="18.4" customHeight="1" s="47">
+    <row r="13" ht="18.4" customHeight="1" s="49">
       <c r="A13" s="13" t="inlineStr">
         <is>
           <t>Night1</t>
@@ -1933,7 +1939,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18.4" customHeight="1" s="47">
+    <row r="14" ht="18.4" customHeight="1" s="49">
       <c r="A14" s="13" t="inlineStr">
         <is>
           <t>Bar Lounge1</t>
@@ -1958,7 +1964,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="18.4" customHeight="1" s="47">
+    <row r="15" ht="18.4" customHeight="1" s="49">
       <c r="A15" s="13" t="inlineStr">
         <is>
           <t>Bar Lounge1</t>
@@ -1983,7 +1989,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="18.4" customHeight="1" s="47">
+    <row r="16" ht="18.4" customHeight="1" s="49">
       <c r="A16" s="13" t="inlineStr">
         <is>
           <t>Bar Lounge1</t>
@@ -2008,7 +2014,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="18.4" customHeight="1" s="47">
+    <row r="17" ht="18.4" customHeight="1" s="49">
       <c r="A17" s="13" t="inlineStr">
         <is>
           <t>Work Study1</t>
@@ -2029,7 +2035,7 @@
       </c>
       <c r="E17" s="18" t="n"/>
     </row>
-    <row r="18" ht="18.4" customHeight="1" s="47">
+    <row r="18" ht="18.4" customHeight="1" s="49">
       <c r="A18" s="13" t="inlineStr">
         <is>
           <t>Reading1</t>
@@ -2054,7 +2060,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="18.4" customHeight="1" s="47">
+    <row r="19" ht="18.4" customHeight="1" s="49">
       <c r="A19" s="13" t="inlineStr">
         <is>
           <t>Reading1</t>
@@ -2115,18 +2121,18 @@
     <col width="19.6016" customWidth="1" style="40" min="6" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.2" customHeight="1" s="47">
+    <row r="1" ht="18.2" customHeight="1" s="49">
       <c r="A1" s="20" t="inlineStr">
         <is>
           <t>表1</t>
         </is>
       </c>
-      <c r="B1" s="48" t="n"/>
-      <c r="C1" s="48" t="n"/>
-      <c r="D1" s="48" t="n"/>
-      <c r="E1" s="49" t="n"/>
-    </row>
-    <row r="2" ht="15.1" customHeight="1" s="47">
+      <c r="B1" s="50" t="n"/>
+      <c r="C1" s="50" t="n"/>
+      <c r="D1" s="50" t="n"/>
+      <c r="E1" s="51" t="n"/>
+    </row>
+    <row r="2" ht="15.1" customHeight="1" s="49">
       <c r="A2" s="21" t="inlineStr">
         <is>
           <t>Style</t>
@@ -2149,113 +2155,133 @@
       </c>
       <c r="E2" s="23" t="n"/>
     </row>
-    <row r="3" ht="14.85" customHeight="1" s="47">
+    <row r="3" ht="14.85" customHeight="1" s="49">
       <c r="A3" s="24" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_BossaNova_4-4</t>
         </is>
       </c>
       <c r="B3" s="25" t="n">
-        <v>1200000</v>
+        <v>746467</v>
       </c>
       <c r="C3" s="27" t="n">
-        <v>38625</v>
+        <v>36588</v>
       </c>
       <c r="D3" s="27" t="n">
-        <v>1161375</v>
+        <v>709879</v>
       </c>
       <c r="E3" s="27" t="n"/>
     </row>
-    <row r="4" ht="14.65" customHeight="1" s="47">
+    <row r="4" ht="14.65" customHeight="1" s="49">
       <c r="A4" s="28" t="inlineStr">
         <is>
           <t>Pf-Bs-Perc_BossaNova_4-4</t>
         </is>
       </c>
       <c r="B4" s="29" t="n">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="31" t="n">
-        <v>76230</v>
+        <v>0</v>
       </c>
       <c r="D4" s="31" t="n">
-        <v>223770</v>
+        <v>0</v>
       </c>
       <c r="E4" s="31" t="n"/>
     </row>
-    <row r="5" ht="14.65" customHeight="1" s="47">
+    <row r="5" ht="14.65" customHeight="1" s="49">
       <c r="A5" s="28" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_Samba_4-4</t>
         </is>
       </c>
       <c r="B5" s="34" t="n">
-        <v>270000</v>
+        <v>161600</v>
       </c>
       <c r="C5" s="31" t="n">
-        <v>35701</v>
+        <v>17670</v>
       </c>
       <c r="D5" s="31" t="n">
-        <v>234299</v>
+        <v>143930</v>
       </c>
       <c r="E5" s="31" t="n"/>
     </row>
-    <row r="6" ht="14.65" customHeight="1" s="47">
+    <row r="6" ht="14.65" customHeight="1" s="49">
       <c r="A6" s="28" t="inlineStr">
         <is>
           <t>Pf-Gt-Bs-Ds_MediumSwing_4-4</t>
         </is>
       </c>
       <c r="B6" s="34" t="n">
-        <v>6000</v>
+        <v>43</v>
       </c>
       <c r="C6" s="31" t="n">
-        <v>2939</v>
+        <v>0</v>
       </c>
       <c r="D6" s="31" t="n">
-        <v>3061</v>
+        <v>43</v>
       </c>
       <c r="E6" s="31" t="n"/>
     </row>
-    <row r="7" ht="14.65" customHeight="1" s="47">
+    <row r="7" ht="14.65" customHeight="1" s="49">
       <c r="A7" s="28" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_MediumSwing_4-4</t>
         </is>
       </c>
       <c r="B7" s="34" t="n">
-        <v>17000</v>
+        <v>74844</v>
       </c>
       <c r="C7" s="31" t="n">
-        <v>11505</v>
+        <v>33579</v>
       </c>
       <c r="D7" s="31" t="n">
-        <v>5495</v>
+        <v>41265</v>
       </c>
       <c r="E7" s="31" t="n"/>
     </row>
-    <row r="8" ht="14.35" customHeight="1" s="47">
-      <c r="A8" s="33" t="n"/>
-      <c r="B8" s="34" t="n"/>
-      <c r="C8" s="31" t="n"/>
-      <c r="D8" s="31" t="n"/>
+    <row r="8" ht="14.35" customHeight="1" s="49">
+      <c r="A8" s="28" t="inlineStr">
+        <is>
+          <t>Pf-Bs-Ds_UpBossaNova_4-4</t>
+        </is>
+      </c>
+      <c r="B8" s="34" t="n">
+        <v>351460</v>
+      </c>
+      <c r="C8" s="31" t="n">
+        <v>18315</v>
+      </c>
+      <c r="D8" s="31" t="n">
+        <v>333145</v>
+      </c>
       <c r="E8" s="31" t="n"/>
     </row>
-    <row r="9" ht="14.35" customHeight="1" s="47">
-      <c r="A9" s="33" t="n"/>
-      <c r="B9" s="34" t="n"/>
-      <c r="C9" s="31" t="n"/>
-      <c r="D9" s="31" t="n"/>
+    <row r="9" ht="14.35" customHeight="1" s="49">
+      <c r="A9" s="28" t="inlineStr">
+        <is>
+          <t>Pf-Bs-Ds_UpSwing_4-4</t>
+        </is>
+      </c>
+      <c r="B9" s="34" t="n">
+        <v>176973</v>
+      </c>
+      <c r="C9" s="31" t="n">
+        <v>13638</v>
+      </c>
+      <c r="D9" s="31" t="n">
+        <v>163335</v>
+      </c>
       <c r="E9" s="31" t="n"/>
     </row>
-    <row r="10" ht="14.35" customHeight="1" s="47">
+    <row r="10" ht="14.35" customHeight="1" s="49">
       <c r="A10" s="33" t="n"/>
       <c r="B10" s="34" t="n"/>
       <c r="C10" s="31" t="n"/>
       <c r="D10" s="31" t="n"/>
       <c r="E10" s="31" t="n"/>
     </row>
-    <row r="11" ht="14.35" customHeight="1" s="47">
+    <row r="11" ht="14.35" customHeight="1" s="49">
       <c r="A11" s="33" t="n"/>
       <c r="B11" s="34" t="n"/>
       <c r="C11" s="31" t="n"/>
@@ -2293,9 +2319,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" style="47" min="1" max="1"/>
-    <col width="20" customWidth="1" style="47" min="2" max="2"/>
-    <col width="20" customWidth="1" style="47" min="3" max="3"/>
+    <col width="20" customWidth="1" style="49" min="1" max="1"/>
+    <col width="20" customWidth="1" style="49" min="2" max="2"/>
+    <col width="20" customWidth="1" style="49" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2317,7 +2343,7 @@
         </is>
       </c>
       <c r="B2" s="40" t="n">
-        <v>516</v>
+        <v>785</v>
       </c>
     </row>
     <row r="3">
@@ -2327,7 +2353,7 @@
         </is>
       </c>
       <c r="B3" s="40" t="n">
-        <v>712</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -2337,7 +2363,7 @@
         </is>
       </c>
       <c r="B4" s="40" t="n">
-        <v>537</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5">
@@ -2347,7 +2373,7 @@
         </is>
       </c>
       <c r="B5" s="40" t="n">
-        <v>546</v>
+        <v>774</v>
       </c>
     </row>
     <row r="6">
@@ -2357,7 +2383,7 @@
         </is>
       </c>
       <c r="B6" s="40" t="n">
-        <v>805</v>
+        <v>783</v>
       </c>
     </row>
     <row r="7">
@@ -2367,7 +2393,7 @@
         </is>
       </c>
       <c r="B7" s="40" t="n">
-        <v>803</v>
+        <v>546</v>
       </c>
     </row>
     <row r="8">
@@ -2377,7 +2403,7 @@
         </is>
       </c>
       <c r="B8" s="40" t="n">
-        <v>794</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9">
@@ -2387,7 +2413,7 @@
         </is>
       </c>
       <c r="B9" s="40" t="n">
-        <v>787</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -2401,7 +2427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2409,66 +2435,82 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" style="47" min="1" max="1"/>
-    <col width="25" customWidth="1" style="47" min="2" max="2"/>
-    <col width="25" customWidth="1" style="47" min="3" max="3"/>
-    <col width="25" customWidth="1" style="47" min="4" max="4"/>
-    <col width="25" customWidth="1" style="47" min="5" max="5"/>
-    <col width="25" customWidth="1" style="47" min="6" max="6"/>
-    <col width="25" customWidth="1" style="47" min="7" max="7"/>
+    <col width="25" customWidth="1" style="49" min="1" max="1"/>
+    <col width="25" customWidth="1" style="49" min="2" max="2"/>
+    <col width="25" customWidth="1" style="49" min="3" max="3"/>
+    <col width="25" customWidth="1" style="49" min="4" max="4"/>
+    <col width="25" customWidth="1" style="49" min="5" max="5"/>
+    <col width="25" customWidth="1" style="49" min="6" max="6"/>
+    <col width="25" customWidth="1" style="49" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="50" t="inlineStr">
+      <c r="B1" s="52" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_BossaNova_4-4</t>
         </is>
       </c>
-      <c r="C1" s="50" t="inlineStr">
+      <c r="C1" s="52" t="inlineStr">
         <is>
           <t>Pf-Bs-Perc_BossaNova_4-4</t>
         </is>
       </c>
-      <c r="D1" s="50" t="inlineStr">
+      <c r="D1" s="52" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_Samba_4-4</t>
         </is>
       </c>
-      <c r="E1" s="50" t="inlineStr">
+      <c r="E1" s="52" t="inlineStr">
         <is>
           <t>Pf-Gt-Bs-Ds_MediumSwing_4-4</t>
         </is>
       </c>
-      <c r="F1" s="50" t="inlineStr">
+      <c r="F1" s="52" t="inlineStr">
         <is>
           <t>Pf-Bs-Ds_MediumSwing_4-4</t>
         </is>
       </c>
+      <c r="G1" s="52" t="inlineStr">
+        <is>
+          <t>Pf-Bs-Ds_UpBossaNova_4-4</t>
+        </is>
+      </c>
+      <c r="H1" s="52" t="inlineStr">
+        <is>
+          <t>Pf-Bs-Ds_UpSwing_4-4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="50" t="inlineStr">
+      <c r="A2" s="52" t="inlineStr">
         <is>
           <t>Cafe4</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="H2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="50" t="inlineStr">
+      <c r="A3" s="52" t="inlineStr">
         <is>
           <t>CafeUp1</t>
         </is>
@@ -2477,73 +2519,91 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="52" t="inlineStr">
+        <is>
+          <t>CafeSlow1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>21</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>9</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="52" t="inlineStr">
+        <is>
+          <t>Morning1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>5</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="50" t="inlineStr">
-        <is>
-          <t>CafeSlow1</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>10</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="52" t="inlineStr">
+        <is>
+          <t>Night1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>9</v>
       </c>
-      <c r="C4" t="n">
-        <v>16</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="50" t="inlineStr">
-        <is>
-          <t>Morning1</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="50" t="inlineStr">
-        <is>
-          <t>Night1</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>9</v>
@@ -2552,11 +2612,17 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="50" t="inlineStr">
+      <c r="A7" s="52" t="inlineStr">
         <is>
           <t>BarLounge1</t>
         </is>
@@ -2565,20 +2631,26 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="50" t="inlineStr">
+      <c r="A8" s="52" t="inlineStr">
         <is>
           <t>WorkStudy1</t>
         </is>
@@ -2587,10 +2659,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -2598,9 +2670,15 @@
       <c r="F8" t="n">
         <v>0</v>
       </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="50" t="inlineStr">
+      <c r="A9" s="52" t="inlineStr">
         <is>
           <t>Reading1</t>
         </is>
@@ -2609,16 +2687,22 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>3</v>
+        <v>24</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>